<commit_message>
Update to use Instance Name column instead of Count - one row per instance
</commit_message>
<xml_diff>
--- a/AWS_Sample.xlsx
+++ b/AWS_Sample.xlsx
@@ -397,17 +397,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>Instance Name</v>
+      </c>
+      <c r="B1" t="str">
         <v>Instance Type</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Count</v>
       </c>
       <c r="C1" t="str">
         <v>Region</v>
@@ -424,10 +424,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>web-server-01</v>
+      </c>
+      <c r="B2" t="str">
         <v>t2.micro</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
       </c>
       <c r="C2" t="str">
         <v>us-east-1</v>
@@ -444,19 +444,19 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>m5.xlarge</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
+        <v>web-server-02</v>
+      </c>
+      <c r="B3" t="str">
+        <v>t2.micro</v>
       </c>
       <c r="C3" t="str">
-        <v>us-west-2</v>
+        <v>us-east-1</v>
       </c>
       <c r="D3" t="str">
-        <v>Windows</v>
+        <v>Linux</v>
       </c>
       <c r="E3">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="F3" t="str">
         <v>SSD</v>
@@ -464,19 +464,19 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>c5.2xlarge</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
+        <v>app-server-01</v>
+      </c>
+      <c r="B4" t="str">
+        <v>m5.xlarge</v>
       </c>
       <c r="C4" t="str">
-        <v>ap-southeast-1</v>
+        <v>us-west-2</v>
       </c>
       <c r="D4" t="str">
-        <v>Linux</v>
+        <v>Windows</v>
       </c>
       <c r="E4">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="F4" t="str">
         <v>SSD</v>
@@ -484,19 +484,19 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>r5.large</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
+        <v>api-server-01</v>
+      </c>
+      <c r="B5" t="str">
+        <v>c5.2xlarge</v>
       </c>
       <c r="C5" t="str">
-        <v>eu-west-1</v>
+        <v>ap-southeast-1</v>
       </c>
       <c r="D5" t="str">
         <v>Linux</v>
       </c>
       <c r="E5">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="F5" t="str">
         <v>SSD</v>
@@ -504,27 +504,107 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
+        <v>api-server-02</v>
+      </c>
+      <c r="B6" t="str">
+        <v>c5.2xlarge</v>
+      </c>
+      <c r="C6" t="str">
+        <v>ap-southeast-1</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Linux</v>
+      </c>
+      <c r="E6">
+        <v>200</v>
+      </c>
+      <c r="F6" t="str">
+        <v>SSD</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>api-server-03</v>
+      </c>
+      <c r="B7" t="str">
+        <v>c5.2xlarge</v>
+      </c>
+      <c r="C7" t="str">
+        <v>ap-southeast-1</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Linux</v>
+      </c>
+      <c r="E7">
+        <v>200</v>
+      </c>
+      <c r="F7" t="str">
+        <v>SSD</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>db-server-01</v>
+      </c>
+      <c r="B8" t="str">
+        <v>r5.large</v>
+      </c>
+      <c r="C8" t="str">
+        <v>eu-west-1</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Linux</v>
+      </c>
+      <c r="E8">
+        <v>300</v>
+      </c>
+      <c r="F8" t="str">
+        <v>SSD</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>db-server-02</v>
+      </c>
+      <c r="B9" t="str">
+        <v>r5.large</v>
+      </c>
+      <c r="C9" t="str">
+        <v>eu-west-1</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Linux</v>
+      </c>
+      <c r="E9">
+        <v>300</v>
+      </c>
+      <c r="F9" t="str">
+        <v>SSD</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>cache-server-01</v>
+      </c>
+      <c r="B10" t="str">
         <v>m6i.2xlarge</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="str">
+      <c r="C10" t="str">
         <v>us-east-1</v>
       </c>
-      <c r="D6" t="str">
-        <v>Linux</v>
-      </c>
-      <c r="E6">
+      <c r="D10" t="str">
+        <v>Linux</v>
+      </c>
+      <c r="E10">
         <v>250</v>
       </c>
-      <c r="F6" t="str">
+      <c r="F10" t="str">
         <v>SSD</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>